<commit_message>
autoReconnect 제거, Log 클래스의 NullPointerException 해결
</commit_message>
<xml_diff>
--- a/Vert.x-Server-Quickstart/API Document.xlsx
+++ b/Vert.x-Server-Quickstart/API Document.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>Function Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+  <si>
+    <t>Function Category</t>
   </si>
   <si>
     <t>Summary</t>
@@ -47,10 +47,13 @@
     <t>Failure Code</t>
   </si>
   <si>
-    <t>샘플</t>
-  </si>
-  <si>
-    <t>기능기능</t>
+    <t>ETC</t>
+  </si>
+  <si>
+    <t>기능 이름</t>
+  </si>
+  <si>
+    <t>요약</t>
   </si>
   <si>
     <t>POST</t>
@@ -112,7 +115,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -152,40 +155,46 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" t="n">
         <v>201.0</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" t="n">
         <v>204.0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>